<commit_message>
version #1; kurzer key ok; grosse letters NOK
</commit_message>
<xml_diff>
--- a/vigenere.xlsx
+++ b/vigenere.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="66">
   <si>
     <t>Asm</t>
   </si>
@@ -136,15 +136,6 @@
     <t>speichern zu tmp</t>
   </si>
   <si>
-    <t>ist schon 0</t>
-  </si>
-  <si>
-    <t>nein, mache weiter</t>
-  </si>
-  <si>
-    <t>ja, tbd</t>
-  </si>
-  <si>
     <t>zähler zurücksetzen</t>
   </si>
   <si>
@@ -160,9 +151,6 @@
     <t>erhöhe buchstaben-taker org</t>
   </si>
   <si>
-    <t>erhöhe buchstaben-tester</t>
-  </si>
-  <si>
     <t>erhöhe speicher-ziel</t>
   </si>
   <si>
@@ -194,6 +182,39 @@
   </si>
   <si>
     <t>Letter in Ziel speichern</t>
+  </si>
+  <si>
+    <t>anzahl buchstaben -1</t>
+  </si>
+  <si>
+    <t>ja, weiter machen</t>
+  </si>
+  <si>
+    <t>nein, somit limit übertreten und zurücksetzen</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>zähle zeichen</t>
+  </si>
+  <si>
+    <t>nimm anzahl zeichen</t>
+  </si>
+  <si>
+    <t>start abziehen</t>
+  </si>
+  <si>
+    <t>anzahl zeichen speichern</t>
+  </si>
+  <si>
+    <t>anzahl buchstaben -1 (weil index 0)</t>
   </si>
 </sst>
 </file>
@@ -601,8 +622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D102"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D102" sqref="D2:D102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,7 +631,7 @@
     <col min="1" max="1" width="9.140625" style="2"/>
     <col min="3" max="3" width="9.140625" style="4"/>
     <col min="4" max="4" width="9.140625" style="6"/>
-    <col min="5" max="5" width="54.28515625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="28.85546875" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -735,11 +756,11 @@
         <v>6</v>
       </c>
       <c r="C6" s="4">
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="D6" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>065</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>22</v>
@@ -760,11 +781,12 @@
         <v>6</v>
       </c>
       <c r="C7" s="4">
-        <v>126</v>
+        <f>C6+26</f>
+        <v>91</v>
       </c>
       <c r="D7" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>126</v>
+        <v>091</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>23</v>
@@ -1019,6 +1041,9 @@
         <f t="shared" si="0"/>
         <v>13999</v>
       </c>
+      <c r="E18" s="8" t="s">
+        <v>61</v>
+      </c>
       <c r="H18" t="s">
         <v>28</v>
       </c>
@@ -1039,6 +1064,9 @@
         <f t="shared" si="0"/>
         <v>1016</v>
       </c>
+      <c r="E19" s="8" t="s">
+        <v>62</v>
+      </c>
       <c r="H19" t="s">
         <v>29</v>
       </c>
@@ -1059,6 +1087,9 @@
         <f t="shared" si="0"/>
         <v>3002</v>
       </c>
+      <c r="E20" s="8" t="s">
+        <v>63</v>
+      </c>
       <c r="H20" t="s">
         <v>30</v>
       </c>
@@ -1079,6 +1110,9 @@
         <f t="shared" si="0"/>
         <v>4001</v>
       </c>
+      <c r="E21" s="8" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
@@ -1096,6 +1130,9 @@
         <f t="shared" si="0"/>
         <v>8001</v>
       </c>
+      <c r="E22" s="8" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
@@ -1103,66 +1140,69 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="2">
+        <f>A3</f>
+        <v>1</v>
+      </c>
+      <c r="D23" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>8001</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C24" s="2">
         <f>A5</f>
         <v>3</v>
       </c>
-      <c r="D23" s="6" t="str">
+      <c r="D24" s="6" t="str">
         <f t="shared" si="0"/>
         <v>1003</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
-        <f t="shared" si="1"/>
-        <v>22</v>
-      </c>
-      <c r="B24" t="s">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
         <v>10</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C25" s="2">
         <f>A37</f>
         <v>35</v>
       </c>
-      <c r="D24" s="6" t="str">
+      <c r="D25" s="6" t="str">
         <f t="shared" si="0"/>
         <v>4035</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
-        <f t="shared" si="1"/>
-        <v>23</v>
-      </c>
-      <c r="B25" t="s">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
         <v>7</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C26" s="2">
         <f>A12</f>
         <v>10</v>
       </c>
-      <c r="D25" s="6" t="str">
+      <c r="D26" s="6" t="str">
         <f t="shared" si="0"/>
         <v>1010</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
-        <f t="shared" si="1"/>
-        <v>24</v>
-      </c>
-      <c r="B26" t="s">
-        <v>10</v>
-      </c>
-      <c r="C26" s="2">
-        <f>A56</f>
-        <v>54</v>
-      </c>
-      <c r="D26" s="6" t="str">
-        <f t="shared" ref="D26:D27" si="2">VLOOKUP(B26,WB,2,FALSE)&amp;TEXT(C26,"000")</f>
-        <v>4054</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1171,103 +1211,100 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C27" s="2">
         <f>A56</f>
         <v>54</v>
       </c>
       <c r="D27" s="6" t="str">
+        <f t="shared" ref="D27:D28" si="2">VLOOKUP(B27,WB,2,FALSE)&amp;TEXT(C27,"000")</f>
+        <v>4054</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="2">
+        <f>A56</f>
+        <v>54</v>
+      </c>
+      <c r="D28" s="6" t="str">
         <f t="shared" si="2"/>
         <v>7054</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
-        <f t="shared" si="1"/>
-        <v>26</v>
-      </c>
-      <c r="B28" t="s">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C29" s="2">
         <f>A11</f>
         <v>9</v>
       </c>
-      <c r="D28" s="6" t="str">
+      <c r="D29" s="6" t="str">
         <f t="shared" si="0"/>
         <v>1009</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
-        <f t="shared" si="1"/>
-        <v>27</v>
-      </c>
-      <c r="B29" t="s">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
         <v>10</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C30" s="2">
         <f>A38</f>
         <v>36</v>
       </c>
-      <c r="D29" s="6" t="str">
+      <c r="D30" s="6" t="str">
         <f t="shared" si="0"/>
         <v>4036</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
-        <f t="shared" si="1"/>
-        <v>28</v>
-      </c>
-      <c r="B30" t="s">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
         <v>7</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C31" s="2">
         <f>A10</f>
         <v>8</v>
       </c>
-      <c r="D30" s="6" t="str">
+      <c r="D31" s="6" t="str">
         <f t="shared" si="0"/>
         <v>1008</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
-        <f t="shared" si="1"/>
-        <v>29</v>
-      </c>
-      <c r="B31" t="s">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
         <v>10</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C32" s="2">
         <f>A47</f>
         <v>45</v>
       </c>
-      <c r="D31" s="6" t="str">
+      <c r="D32" s="6" t="str">
         <f t="shared" si="0"/>
         <v>4045</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
-        <f t="shared" si="1"/>
-        <v>30</v>
-      </c>
-      <c r="B32" t="s">
-        <v>11</v>
-      </c>
-      <c r="C32" s="2">
-        <f>A37</f>
-        <v>35</v>
-      </c>
-      <c r="D32" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>5035</v>
-      </c>
-      <c r="E32" s="8" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1276,7 +1313,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C33" s="2">
         <f>A37</f>
@@ -1284,10 +1321,10 @@
       </c>
       <c r="D33" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>7035</v>
+        <v>5035</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1299,20 +1336,20 @@
         <v>13</v>
       </c>
       <c r="C34" s="2">
-        <f>A44</f>
-        <v>42</v>
+        <f>A37</f>
+        <v>35</v>
       </c>
       <c r="D34" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>7042</v>
+        <v>7035</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
-        <f>A34+1</f>
+        <f t="shared" si="1"/>
         <v>33</v>
       </c>
       <c r="B35" t="s">
@@ -1327,7 +1364,7 @@
         <v>7045</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1347,7 +1384,7 @@
         <v>7054</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1366,7 +1403,7 @@
         <v>1999</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1385,7 +1422,7 @@
         <v>2999</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1405,7 +1442,7 @@
         <v>3004</v>
       </c>
       <c r="E39" s="12" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1465,7 +1502,7 @@
         <v>3005</v>
       </c>
       <c r="E42" s="12" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1485,7 +1522,7 @@
         <v>4006</v>
       </c>
       <c r="E43" s="12" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1505,7 +1542,7 @@
         <v>6006</v>
       </c>
       <c r="E44" s="12" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1525,7 +1562,7 @@
         <v>4007</v>
       </c>
       <c r="E45" s="12" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1545,7 +1582,7 @@
         <v>1007</v>
       </c>
       <c r="E46" s="12" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1564,7 +1601,7 @@
         <v>4999</v>
       </c>
       <c r="E47" s="12" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -1580,7 +1617,7 @@
         <v>36</v>
       </c>
       <c r="D48" s="6" t="str">
-        <f>VLOOKUP(B48,WB,2,FALSE)&amp;TEXT(C48,"000")</f>
+        <f t="shared" ref="D48:D55" si="5">VLOOKUP(B48,WB,2,FALSE)&amp;TEXT(C48,"000")</f>
         <v>7036</v>
       </c>
       <c r="E48" s="8" t="s">
@@ -1600,7 +1637,7 @@
         <v>36</v>
       </c>
       <c r="D49" s="6" t="str">
-        <f>VLOOKUP(B49,WB,2,FALSE)&amp;TEXT(C49,"000")</f>
+        <f t="shared" si="5"/>
         <v>1036</v>
       </c>
       <c r="E49" s="12" t="s">
@@ -1620,7 +1657,7 @@
         <v>9</v>
       </c>
       <c r="D50" s="6" t="str">
-        <f>VLOOKUP(B50,WB,2,FALSE)&amp;TEXT(C50,"000")</f>
+        <f t="shared" si="5"/>
         <v>3009</v>
       </c>
       <c r="E50" s="12" t="s">
@@ -1640,7 +1677,7 @@
         <v>1</v>
       </c>
       <c r="D51" s="6" t="str">
-        <f>VLOOKUP(B51,WB,2,FALSE)&amp;TEXT(C51,"000")</f>
+        <f t="shared" si="5"/>
         <v>3001</v>
       </c>
       <c r="E51" s="12" t="s">
@@ -1660,7 +1697,7 @@
         <v>6</v>
       </c>
       <c r="D52" s="6" t="str">
-        <f>VLOOKUP(B52,WB,2,FALSE)&amp;TEXT(C52,"000")</f>
+        <f t="shared" si="5"/>
         <v>4006</v>
       </c>
       <c r="E52" s="12" t="s">
@@ -1680,11 +1717,11 @@
         <v>6</v>
       </c>
       <c r="D53" s="6" t="str">
-        <f>VLOOKUP(B53,WB,2,FALSE)&amp;TEXT(C53,"000")</f>
+        <f t="shared" si="5"/>
         <v>6006</v>
       </c>
       <c r="E53" s="12" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -1696,35 +1733,35 @@
         <v>11</v>
       </c>
       <c r="C54" s="2">
+        <f>A59</f>
+        <v>57</v>
+      </c>
+      <c r="D54" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v>5057</v>
+      </c>
+      <c r="E54" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="2">
+        <f t="shared" si="1"/>
+        <v>53</v>
+      </c>
+      <c r="B55" t="s">
+        <v>11</v>
+      </c>
+      <c r="C55" s="2">
         <f>A56</f>
         <v>54</v>
       </c>
-      <c r="D54" s="6" t="str">
-        <f>VLOOKUP(B54,WB,2,FALSE)&amp;TEXT(C54,"000")</f>
+      <c r="D55" s="6" t="str">
+        <f t="shared" si="5"/>
         <v>5054</v>
       </c>
-      <c r="E54" s="12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="2">
-        <f t="shared" si="1"/>
-        <v>53</v>
-      </c>
-      <c r="B55" t="s">
-        <v>11</v>
-      </c>
-      <c r="C55" s="2">
-        <f>A59</f>
-        <v>57</v>
-      </c>
-      <c r="D55" s="6" t="str">
-        <f>VLOOKUP(B55,WB,2,FALSE)&amp;TEXT(C55,"000")</f>
-        <v>5057</v>
-      </c>
       <c r="E55" s="12" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -1755,12 +1792,12 @@
         <v>11</v>
       </c>
       <c r="C57" s="2">
-        <f>A33</f>
-        <v>31</v>
+        <f>A34</f>
+        <v>32</v>
       </c>
       <c r="D57" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>5031</v>
+        <v>5032</v>
       </c>
       <c r="E57" s="8" t="s">
         <v>32</v>
@@ -1799,11 +1836,11 @@
         <v>9</v>
       </c>
       <c r="D59" s="6" t="str">
-        <f t="shared" ref="D59:D60" si="5">VLOOKUP(B59,WB,2,FALSE)&amp;TEXT(C59,"000")</f>
+        <f t="shared" ref="D59:D60" si="6">VLOOKUP(B59,WB,2,FALSE)&amp;TEXT(C59,"000")</f>
         <v>1009</v>
       </c>
       <c r="E59" s="8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -1819,11 +1856,11 @@
         <v>36</v>
       </c>
       <c r="D60" s="6" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4036</v>
       </c>
       <c r="E60" s="8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -1839,11 +1876,11 @@
         <v>54</v>
       </c>
       <c r="D61" s="6" t="str">
-        <f>VLOOKUP(B61,WB,2,FALSE)&amp;TEXT(C61,"000")</f>
+        <f t="shared" ref="D61:D102" si="7">VLOOKUP(B61,WB,2,FALSE)&amp;TEXT(C61,"000")</f>
         <v>5054</v>
       </c>
       <c r="E61" s="12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -1856,7 +1893,7 @@
       </c>
       <c r="C62" s="2"/>
       <c r="D62" s="6" t="str">
-        <f>VLOOKUP(B62,WB,2,FALSE)&amp;TEXT(C62,"000")</f>
+        <f t="shared" si="7"/>
         <v>000</v>
       </c>
       <c r="E62" s="12"/>
@@ -1871,7 +1908,7 @@
       </c>
       <c r="C63" s="2"/>
       <c r="D63" s="6" t="str">
-        <f>VLOOKUP(B63,WB,2,FALSE)&amp;TEXT(C63,"000")</f>
+        <f t="shared" si="7"/>
         <v>000</v>
       </c>
       <c r="E63" s="12"/>
@@ -1886,7 +1923,7 @@
       </c>
       <c r="C64" s="2"/>
       <c r="D64" s="6" t="str">
-        <f>VLOOKUP(B64,WB,2,FALSE)&amp;TEXT(C64,"000")</f>
+        <f t="shared" si="7"/>
         <v>000</v>
       </c>
       <c r="E64" s="12"/>
@@ -1901,7 +1938,7 @@
       </c>
       <c r="C65" s="2"/>
       <c r="D65" s="6" t="str">
-        <f>VLOOKUP(B65,WB,2,FALSE)&amp;TEXT(C65,"000")</f>
+        <f t="shared" si="7"/>
         <v>000</v>
       </c>
       <c r="E65" s="12"/>
@@ -1916,7 +1953,7 @@
       </c>
       <c r="C66" s="2"/>
       <c r="D66" s="6" t="str">
-        <f>VLOOKUP(B66,WB,2,FALSE)&amp;TEXT(C66,"000")</f>
+        <f t="shared" si="7"/>
         <v>000</v>
       </c>
       <c r="E66" s="12"/>
@@ -1931,7 +1968,7 @@
       </c>
       <c r="C67" s="2"/>
       <c r="D67" s="6" t="str">
-        <f>VLOOKUP(B67,WB,2,FALSE)&amp;TEXT(C67,"000")</f>
+        <f t="shared" si="7"/>
         <v>000</v>
       </c>
       <c r="E67" s="12"/>
@@ -1946,7 +1983,7 @@
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="6" t="str">
-        <f>VLOOKUP(B68,WB,2,FALSE)&amp;TEXT(C68,"000")</f>
+        <f t="shared" si="7"/>
         <v>000</v>
       </c>
       <c r="E68" s="12"/>
@@ -1961,7 +1998,7 @@
       </c>
       <c r="C69" s="2"/>
       <c r="D69" s="6" t="str">
-        <f>VLOOKUP(B69,WB,2,FALSE)&amp;TEXT(C69,"000")</f>
+        <f t="shared" si="7"/>
         <v>000</v>
       </c>
       <c r="E69" s="12"/>
@@ -1976,7 +2013,7 @@
       </c>
       <c r="C70" s="2"/>
       <c r="D70" s="6" t="str">
-        <f>VLOOKUP(B70,WB,2,FALSE)&amp;TEXT(C70,"000")</f>
+        <f t="shared" si="7"/>
         <v>000</v>
       </c>
       <c r="E70" s="12"/>
@@ -1991,7 +2028,7 @@
       </c>
       <c r="C71" s="2"/>
       <c r="D71" s="6" t="str">
-        <f>VLOOKUP(B71,WB,2,FALSE)&amp;TEXT(C71,"000")</f>
+        <f t="shared" si="7"/>
         <v>000</v>
       </c>
       <c r="E71" s="12"/>
@@ -2005,11 +2042,14 @@
         <v>6</v>
       </c>
       <c r="C72" s="4">
-        <v>101</v>
+        <v>70</v>
       </c>
       <c r="D72" s="6" t="str">
-        <f>VLOOKUP(B72,WB,2,FALSE)&amp;TEXT(C72,"000")</f>
-        <v>101</v>
+        <f t="shared" si="7"/>
+        <v>070</v>
+      </c>
+      <c r="E72" s="8" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -2021,11 +2061,14 @@
         <v>6</v>
       </c>
       <c r="C73" s="4">
-        <v>101</v>
+        <v>70</v>
       </c>
       <c r="D73" s="6" t="str">
-        <f>VLOOKUP(B73,WB,2,FALSE)&amp;TEXT(C73,"000")</f>
-        <v>101</v>
+        <f t="shared" si="7"/>
+        <v>070</v>
+      </c>
+      <c r="E73" s="8" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -2037,11 +2080,14 @@
         <v>6</v>
       </c>
       <c r="C74" s="4">
-        <v>101</v>
+        <v>72</v>
       </c>
       <c r="D74" s="6" t="str">
-        <f>VLOOKUP(B74,WB,2,FALSE)&amp;TEXT(C74,"000")</f>
-        <v>101</v>
+        <f t="shared" si="7"/>
+        <v>072</v>
+      </c>
+      <c r="E74" s="8" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -2053,11 +2099,14 @@
         <v>6</v>
       </c>
       <c r="C75" s="4">
-        <v>101</v>
+        <v>83</v>
       </c>
       <c r="D75" s="6" t="str">
-        <f>VLOOKUP(B75,WB,2,FALSE)&amp;TEXT(C75,"000")</f>
-        <v>101</v>
+        <f t="shared" si="7"/>
+        <v>083</v>
+      </c>
+      <c r="E75" s="8" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -2069,7 +2118,7 @@
         <v>6</v>
       </c>
       <c r="D76" s="6" t="str">
-        <f>VLOOKUP(B76,WB,2,FALSE)&amp;TEXT(C76,"000")</f>
+        <f t="shared" si="7"/>
         <v>000</v>
       </c>
     </row>
@@ -2082,7 +2131,7 @@
         <v>6</v>
       </c>
       <c r="D77" s="6" t="str">
-        <f>VLOOKUP(B77,WB,2,FALSE)&amp;TEXT(C77,"000")</f>
+        <f t="shared" si="7"/>
         <v>000</v>
       </c>
     </row>
@@ -2095,7 +2144,7 @@
         <v>6</v>
       </c>
       <c r="D78" s="6" t="str">
-        <f>VLOOKUP(B78,WB,2,FALSE)&amp;TEXT(C78,"000")</f>
+        <f t="shared" si="7"/>
         <v>000</v>
       </c>
     </row>
@@ -2108,7 +2157,7 @@
         <v>6</v>
       </c>
       <c r="D79" s="6" t="str">
-        <f>VLOOKUP(B79,WB,2,FALSE)&amp;TEXT(C79,"000")</f>
+        <f t="shared" si="7"/>
         <v>000</v>
       </c>
     </row>
@@ -2121,11 +2170,11 @@
         <v>6</v>
       </c>
       <c r="D80" s="6" t="str">
-        <f>VLOOKUP(B80,WB,2,FALSE)&amp;TEXT(C80,"000")</f>
-        <v>000</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>000</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="11">
         <f t="shared" si="1"/>
         <v>79</v>
@@ -2134,11 +2183,11 @@
         <v>6</v>
       </c>
       <c r="D81" s="6" t="str">
-        <f>VLOOKUP(B81,WB,2,FALSE)&amp;TEXT(C81,"000")</f>
-        <v>000</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>000</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="11">
         <f t="shared" si="1"/>
         <v>80</v>
@@ -2147,14 +2196,18 @@
         <v>6</v>
       </c>
       <c r="C82" s="4">
-        <v>101</v>
+        <v>65</v>
       </c>
       <c r="D82" s="6" t="str">
-        <f>VLOOKUP(B82,WB,2,FALSE)&amp;TEXT(C82,"000")</f>
-        <v>101</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>065</v>
+      </c>
+      <c r="E82" s="8">
+        <f>C82-65+C72</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="11">
         <f t="shared" si="1"/>
         <v>81</v>
@@ -2163,14 +2216,18 @@
         <v>6</v>
       </c>
       <c r="C83" s="4">
-        <v>101</v>
+        <v>66</v>
       </c>
       <c r="D83" s="6" t="str">
-        <f>VLOOKUP(B83,WB,2,FALSE)&amp;TEXT(C83,"000")</f>
-        <v>101</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>066</v>
+      </c>
+      <c r="E83" s="8">
+        <f>C83-65+C73</f>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="11">
         <f t="shared" si="1"/>
         <v>82</v>
@@ -2179,14 +2236,18 @@
         <v>6</v>
       </c>
       <c r="C84" s="4">
-        <v>102</v>
+        <v>67</v>
       </c>
       <c r="D84" s="6" t="str">
-        <f>VLOOKUP(B84,WB,2,FALSE)&amp;TEXT(C84,"000")</f>
-        <v>102</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>067</v>
+      </c>
+      <c r="E84" s="8">
+        <f>C84-65+C74</f>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="11">
         <f t="shared" si="1"/>
         <v>83</v>
@@ -2195,14 +2256,18 @@
         <v>6</v>
       </c>
       <c r="C85" s="4">
-        <v>102</v>
+        <v>68</v>
       </c>
       <c r="D85" s="6" t="str">
-        <f>VLOOKUP(B85,WB,2,FALSE)&amp;TEXT(C85,"000")</f>
-        <v>102</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>068</v>
+      </c>
+      <c r="E85" s="8">
+        <f>C85-65+C75</f>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="11">
         <f t="shared" si="1"/>
         <v>84</v>
@@ -2211,14 +2276,18 @@
         <v>6</v>
       </c>
       <c r="C86" s="4">
-        <v>101</v>
+        <v>65</v>
       </c>
       <c r="D86" s="6" t="str">
-        <f>VLOOKUP(B86,WB,2,FALSE)&amp;TEXT(C86,"000")</f>
-        <v>101</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>065</v>
+      </c>
+      <c r="E86" s="8">
+        <f>C86-65+C72</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="11">
         <f t="shared" si="1"/>
         <v>85</v>
@@ -2227,14 +2296,18 @@
         <v>6</v>
       </c>
       <c r="C87" s="4">
-        <v>102</v>
+        <v>65</v>
       </c>
       <c r="D87" s="6" t="str">
-        <f>VLOOKUP(B87,WB,2,FALSE)&amp;TEXT(C87,"000")</f>
-        <v>102</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>065</v>
+      </c>
+      <c r="E87" s="8">
+        <f>C87-65+C73</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="11">
         <f t="shared" si="1"/>
         <v>86</v>
@@ -2243,11 +2316,11 @@
         <v>6</v>
       </c>
       <c r="D88" s="6" t="str">
-        <f>VLOOKUP(B88,WB,2,FALSE)&amp;TEXT(C88,"000")</f>
-        <v>000</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>000</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <f t="shared" si="1"/>
         <v>87</v>
@@ -2256,11 +2329,11 @@
         <v>6</v>
       </c>
       <c r="D89" s="6" t="str">
-        <f>VLOOKUP(B89,WB,2,FALSE)&amp;TEXT(C89,"000")</f>
-        <v>000</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>000</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <f t="shared" si="1"/>
         <v>88</v>
@@ -2269,11 +2342,11 @@
         <v>6</v>
       </c>
       <c r="D90" s="6" t="str">
-        <f>VLOOKUP(B90,WB,2,FALSE)&amp;TEXT(C90,"000")</f>
-        <v>000</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>000</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <f t="shared" si="1"/>
         <v>89</v>
@@ -2282,11 +2355,11 @@
         <v>6</v>
       </c>
       <c r="D91" s="6" t="str">
-        <f>VLOOKUP(B91,WB,2,FALSE)&amp;TEXT(C91,"000")</f>
-        <v>000</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>000</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <f t="shared" si="1"/>
         <v>90</v>
@@ -2295,137 +2368,137 @@
         <v>6</v>
       </c>
       <c r="D92" s="6" t="str">
-        <f>VLOOKUP(B92,WB,2,FALSE)&amp;TEXT(C92,"000")</f>
-        <v>000</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>000</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
-        <f t="shared" ref="A93:A102" si="6">A92+1</f>
+        <f t="shared" ref="A93:A102" si="8">A92+1</f>
         <v>91</v>
       </c>
       <c r="B93" t="s">
         <v>6</v>
       </c>
       <c r="D93" s="6" t="str">
-        <f>VLOOKUP(B93,WB,2,FALSE)&amp;TEXT(C93,"000")</f>
-        <v>000</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>000</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>92</v>
       </c>
       <c r="B94" t="s">
         <v>6</v>
       </c>
       <c r="D94" s="6" t="str">
-        <f>VLOOKUP(B94,WB,2,FALSE)&amp;TEXT(C94,"000")</f>
-        <v>000</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>000</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>93</v>
       </c>
       <c r="B95" t="s">
         <v>6</v>
       </c>
       <c r="D95" s="6" t="str">
-        <f>VLOOKUP(B95,WB,2,FALSE)&amp;TEXT(C95,"000")</f>
-        <v>000</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>000</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>94</v>
       </c>
       <c r="B96" t="s">
         <v>6</v>
       </c>
       <c r="D96" s="6" t="str">
-        <f>VLOOKUP(B96,WB,2,FALSE)&amp;TEXT(C96,"000")</f>
+        <f t="shared" si="7"/>
         <v>000</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>95</v>
       </c>
       <c r="B97" t="s">
         <v>6</v>
       </c>
       <c r="D97" s="6" t="str">
-        <f>VLOOKUP(B97,WB,2,FALSE)&amp;TEXT(C97,"000")</f>
+        <f t="shared" si="7"/>
         <v>000</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>96</v>
       </c>
       <c r="B98" t="s">
         <v>6</v>
       </c>
       <c r="D98" s="6" t="str">
-        <f>VLOOKUP(B98,WB,2,FALSE)&amp;TEXT(C98,"000")</f>
+        <f t="shared" si="7"/>
         <v>000</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>97</v>
       </c>
       <c r="B99" t="s">
         <v>6</v>
       </c>
       <c r="D99" s="6" t="str">
-        <f>VLOOKUP(B99,WB,2,FALSE)&amp;TEXT(C99,"000")</f>
+        <f t="shared" si="7"/>
         <v>000</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>98</v>
       </c>
       <c r="B100" t="s">
         <v>6</v>
       </c>
       <c r="D100" s="6" t="str">
-        <f>VLOOKUP(B100,WB,2,FALSE)&amp;TEXT(C100,"000")</f>
+        <f t="shared" si="7"/>
         <v>000</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>99</v>
       </c>
       <c r="B101" t="s">
         <v>6</v>
       </c>
       <c r="D101" s="6" t="str">
-        <f>VLOOKUP(B101,WB,2,FALSE)&amp;TEXT(C101,"000")</f>
+        <f t="shared" si="7"/>
         <v>000</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>100</v>
       </c>
       <c r="B102" t="s">
         <v>6</v>
       </c>
       <c r="D102" s="6" t="str">
-        <f>VLOOKUP(B102,WB,2,FALSE)&amp;TEXT(C102,"000")</f>
+        <f t="shared" si="7"/>
         <v>000</v>
       </c>
     </row>

</xml_diff>